<commit_message>
[localdb] - minor adjustments to the generated SQL and console output.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/localdb/artifact/data/localdb.data.xlsx
+++ b/examples/localdb/artifact/data/localdb.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/examples/localdb/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9EEA73-13CC-3146-A351-EB094E551E06}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87E4156-E323-2946-B9DA-E8E8E062C5CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15880" yWindow="2640" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="8380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>true</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>nexial.delayBetweenStepsMs</t>
+  </si>
+  <si>
+    <t>nexial.browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
   </si>
 </sst>
 </file>
@@ -562,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA196"/>
+  <dimension ref="A1:AAA197"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -609,29 +615,38 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="HA4" s="4"/>
-      <c r="AAA4" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="HA4" s="6"/>
+      <c r="AAA4" s="6"/>
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703" ht="23" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
-    <row r="7" spans="1:703" ht="23" customHeight="1"/>
+    <row r="7" spans="1:703" ht="23" customHeight="1">
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
     <row r="8" spans="1:703" ht="23" customHeight="1"/>
     <row r="9" spans="1:703" ht="23" customHeight="1"/>
     <row r="10" spans="1:703" ht="23" customHeight="1"/>
@@ -821,6 +836,7 @@
     <row r="194" ht="23" customHeight="1"/>
     <row r="195" ht="23" customHeight="1"/>
     <row r="196" ht="23" customHeight="1"/>
+    <row r="197" ht="23" customHeight="1"/>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>